<commit_message>
Progress with setting up analyses
</commit_message>
<xml_diff>
--- a/Wheat/RawDatafiles/Canopy.xlsx
+++ b/Wheat/RawDatafiles/Canopy.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="19464" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="19464" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PlotNDVI" sheetId="1" r:id="rId1"/>
     <sheet name="SunScanCover" sheetId="2" r:id="rId2"/>
+    <sheet name="SunScanLAI" sheetId="3" r:id="rId3"/>
+    <sheet name="DestructiveLAI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="13">
   <si>
     <t>Dryland</t>
   </si>
@@ -386,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +553,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
@@ -2950,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4993,4 +4995,2692 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>42292</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.22113744056196674</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.23662383106087267</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.31085533913849878</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.36727748842613372</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.17686763499337835</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.24400392404118273</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.17326710045086186</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.17566952807935729</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.18412142898921086</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.24983837983516272</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.20991946471408571</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.1464835828476411</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.22715035694857363</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.21571260314128074</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.27337278540451199</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.299662110330285</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.24829981382451169</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.22552623389018089</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.26893613419986612</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.12741471295695866</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0.20117971229282544</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.2812686669284884</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0.2349546612522368</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0.13999615653977532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>42297</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.34494519930621348</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.2794493016918756</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.47902669622757754</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.4963218207111314</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.2076216682257665</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.22776184044785727</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.20596807603620965</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.28051737225500584</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.23849629709689119</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.36056971787467185</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.22181939807089521</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.22847409682740999</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.32724445837033656</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.27970946357785786</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.38745303989061142</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0.4316357998780963</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.33276329788219322</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.17105066956373655</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.32780899947731601</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.15616713534959528</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0.33721244139396533</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0.3849863117133413</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0.37628058075354459</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0.22051960842324356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>42307</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.43295594357802819</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.33334694436969325</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.53814876676879064</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.54381837980967895</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.30294426567303678</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.39175013697754979</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.33721347913124006</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.28914206846313467</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.85612947526447125</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.53419669960300875</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.53456966295419306</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.39706296171715449</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.44380918311231826</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.41632923589381188</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.61718034072209882</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0.52180613338209814</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0.46552360260609527</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.46220122248237622</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.39662528124565732</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.33679635215761394</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0.66239118674967712</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0.67551236795019987</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0.6212579712340347</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>0.4357743895676448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.42801550912802189</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.42221083627983419</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.74545347503391157</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.62162287816669204</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.45036399726133663</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.41383830323068949</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.40255299732666555</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.44035539695403714</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.0990696561221978</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.73719471680990789</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.86242136550579462</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.49848037471353146</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.83352510722042739</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.49636669333513772</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.80653105673588854</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.74379116481383722</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.65341304520615306</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.58073108712116683</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.55336674344052894</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.37482777579407622</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1.0295044529399919</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1.0911089154242133</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0.86864803138644908</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0.68488460265090478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>42318</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.61892310348600366</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.54923884900255437</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.0240185141237332</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.85503140654101917</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.64591509274299186</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.65107762513093681</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.61369263205168567</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.58659515765155035</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.6944089490066276</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.2669499674812279</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.3410442807898069</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1.1825887608585</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.85575219895293253</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.61396010676584201</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1.1365363512196485</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.82108964978460963</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.85052900182022539</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.83816518111151805</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.83604797436438916</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.81307658772720726</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1.848806340202372</v>
+      </c>
+      <c r="W9" s="2">
+        <v>2.2360220450793191</v>
+      </c>
+      <c r="X9" s="2">
+        <v>1.5073190148798883</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>1.2316939313809168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.48901493805086577</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.38746850674030875</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.94324314278435484</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.80356370067680383</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.54156790571062241</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.71465181804680411</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.6790356080216956</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.53629876322725334</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.9106137067377496</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.3358656081804323</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.4164795229962139</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1.0841074008026161</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.78370099560942907</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.51328019670854164</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.1207581120705259</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0.89258518222494421</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0.83361162584847182</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.55382699997791685</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.82810668735934312</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.78744422457828434</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1.6383433657116437</v>
+      </c>
+      <c r="W10" s="2">
+        <v>2.1286201267928027</v>
+      </c>
+      <c r="X10" s="2">
+        <v>1.4018610689831474</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>1.239481679208805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>42325</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.75596668898899078</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.58813545368051545</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.3445055125785088</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.95240994485428843</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.83070104399027134</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.85281262035439609</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.71675175614449216</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.7627619060033497</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2.0853915795606275</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.8694989885771278</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.6667856709752726</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.3853212728377235</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1.4222814648524784</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.74636883337616633</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1.442871104420542</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1.1403057417761748</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1.3863749044082632</v>
+      </c>
+      <c r="S11" s="2">
+        <v>1.1198773031954441</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1.1065604326398526</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.81435750596221512</v>
+      </c>
+      <c r="V11" s="2">
+        <v>2.6080681741191931</v>
+      </c>
+      <c r="W11" s="2">
+        <v>2.8468695667849055</v>
+      </c>
+      <c r="X11" s="2">
+        <v>2.0223407083671137</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>1.7436498867137451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>42331</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.57453987147658325</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.51807270553265239</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.2202315765486886</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.8534130527997611</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.78663053907901603</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.85977698168388239</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.74826815285173465</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.82782178379049998</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2.3580961852523958</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.8102034427320866</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1.90855596540885</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.7711981221808653</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1.2279082169609055</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.6875574155374542</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1.2952965101861751</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1.2941182769130184</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1.4136870042957561</v>
+      </c>
+      <c r="S12" s="2">
+        <v>1.081767686393436</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1.1798501932444869</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1.1251005472180773</v>
+      </c>
+      <c r="V12" s="2">
+        <v>2.6302168615299193</v>
+      </c>
+      <c r="W12" s="2">
+        <v>3.2081038286619146</v>
+      </c>
+      <c r="X12" s="2">
+        <v>2.2449355725211406</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>2.3442434142854447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>42338</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.61154086299613541</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.54726714200907833</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.1087219145935183</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.60061893022499691</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.0356284188271925</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.85260751370507926</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.94605997772366135</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.75676954786630968</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.6126978406626451</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.7064628660595003</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2.2254763626849341</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1.9643167710628195</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1.1170376564928239</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.6521543544046573</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.269431340361439</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>1.1303336398103536</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1.5670814546632295</v>
+      </c>
+      <c r="S13" s="2">
+        <v>1.4326231099211468</v>
+      </c>
+      <c r="T13" s="2">
+        <v>1.3624785282276339</v>
+      </c>
+      <c r="U13" s="2">
+        <v>1.429750629940796</v>
+      </c>
+      <c r="V13" s="2">
+        <v>2.9570156660268894</v>
+      </c>
+      <c r="W13" s="2">
+        <v>3.3945976278071326</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3.3746763743185597</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>2.7787333963026408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>42342</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.74184894903377285</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.62185901647579289</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.0737576801034057</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.1298532676353377</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.0659348725735494</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.1532889462736802</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.3876672151704579</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.1062086655459971</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2.885026139688966</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.7962173924250249</v>
+      </c>
+      <c r="L14" s="2">
+        <v>2.1854975495432933</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2.3598981360535967</v>
+      </c>
+      <c r="N14" s="2">
+        <v>1.214214439655674</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.87157690918646968</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.3675468750901976</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.2466753198129061</v>
+      </c>
+      <c r="R14" s="2">
+        <v>1.5906582013077284</v>
+      </c>
+      <c r="S14" s="2">
+        <v>1.7283838139684611</v>
+      </c>
+      <c r="T14" s="2">
+        <v>1.7262820769300711</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1.7308872407780931</v>
+      </c>
+      <c r="V14" s="2">
+        <v>3.4837116925041789</v>
+      </c>
+      <c r="W14" s="2">
+        <v>3.5156710424643256</v>
+      </c>
+      <c r="X14" s="2">
+        <v>3.4737492521199131</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>3.1841153772184194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>42345</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.52884195103316833</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.46957147515175085</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.81946532188385102</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.72721847021203445</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.99215879511646032</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.84824552663345254</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.94048777852240273</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.6644774111833105</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2.5111224767963862</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.4280845862784852</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.7672046289012731</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.8440583043476224</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.1577824069976437</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.64468043912821082</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.95924334648601861</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.0092712856217947</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1.2506408315193362</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.3953968864779331</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1.3739525569663478</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1.602199844404528</v>
+      </c>
+      <c r="V15" s="2">
+        <v>3.2996420880302546</v>
+      </c>
+      <c r="W15" s="2">
+        <v>2.9153502152789912</v>
+      </c>
+      <c r="X15" s="2">
+        <v>2.8848951057511583</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>2.7603256398474558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>42349</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.80835855597888473</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.74025368997286656</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.4276392708198096</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.0994683744268408</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.3241772625151271</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.1873249128162953</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.0703487480023921</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.1676039515987422</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3.4630573832259737</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2.3751232306458188</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2.747321346202753</v>
+      </c>
+      <c r="M16" s="2">
+        <v>2.7718144654193893</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1.6418658105512367</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.0904649500484944</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1.585958555953638</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1.6508402485952516</v>
+      </c>
+      <c r="R16" s="2">
+        <v>2.0299682024001759</v>
+      </c>
+      <c r="S16" s="2">
+        <v>2.140576006614173</v>
+      </c>
+      <c r="T16" s="2">
+        <v>2.3232342548280305</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1.9175497285292167</v>
+      </c>
+      <c r="V16" s="2">
+        <v>4.9451006091459488</v>
+      </c>
+      <c r="W16" s="2">
+        <v>4.9411872352635822</v>
+      </c>
+      <c r="X16" s="2">
+        <v>5.1554809261853478</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>4.4149686606188485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>42352</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.57442847453109824</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5389973731074702</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.91468862500246451</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.82052260697107593</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.81576011382118074</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.76396223062540636</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.82060358424344138</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.74377740356872091</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2.2987194272408962</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.5048488206014194</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1.7798928682845818</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1.7240656056704391</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1.0041977970081672</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.67624159810620799</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1.2555659264535759</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1.0163029907827144</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1.6056941351181808</v>
+      </c>
+      <c r="S17" s="2">
+        <v>1.3989715851474176</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1.5248373228592667</v>
+      </c>
+      <c r="U17" s="2">
+        <v>1.2896714553850028</v>
+      </c>
+      <c r="V17" s="2">
+        <v>3.4056650742861101</v>
+      </c>
+      <c r="W17" s="2">
+        <v>3.346937348519615</v>
+      </c>
+      <c r="X17" s="2">
+        <v>3.0454964257455757</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>3.0837371721447719</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>42359</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.48747490250463688</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.4364604711799136</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.87246948006494396</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.69450572472376548</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.79173817798922086</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.88199497456180254</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.81650436202944499</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.60251935462812101</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2.0344344368644265</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.2621110110900871</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1.7517524190692544</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1.5379913573622954</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.98777322274026536</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.60597056917255809</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1.0426249875115965</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.9063044858774818</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1.4417925022740097</v>
+      </c>
+      <c r="S18" s="2">
+        <v>1.2216591004531649</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1.377307765498597</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1.4850879617935402</v>
+      </c>
+      <c r="V18" s="2">
+        <v>3.1045543596798795</v>
+      </c>
+      <c r="W18" s="2">
+        <v>3.3574906282209751</v>
+      </c>
+      <c r="X18" s="2">
+        <v>3.103726474016566</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>3.0018671264907049</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>42368</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.48268984391385483</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.46825408649459854</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.87860556640841225</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.69445412839854304</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.88675201450685626</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.87151985656225539</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.71272086529581558</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.64546644597257541</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2.1415085096101878</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.4051970056166647</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.6958919556902914</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.7593544006341681</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1.0419400903322631</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.76304063687284729</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1.1759095063226743</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>1.1119320160331072</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1.6009822774875428</v>
+      </c>
+      <c r="S19" s="2">
+        <v>1.4267657582626772</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1.654597622788478</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1.4504847761718931</v>
+      </c>
+      <c r="V19" s="2">
+        <v>3.4111270245062455</v>
+      </c>
+      <c r="W19" s="2">
+        <v>4.0313269502403468</v>
+      </c>
+      <c r="X19" s="2">
+        <v>4.0496820853660447</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>4.0336791234035863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>42375</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.60099776797263793</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.48412800543957868</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.9765139838466721</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.89313866226485816</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.88774720939494789</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.93363838160223112</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.0350183405848756</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.56889747058471252</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2.1893762313843279</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.2755114896650102</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1.8384180704680251</v>
+      </c>
+      <c r="M20" s="2">
+        <v>2.0615255327021265</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1.0224637673818839</v>
+      </c>
+      <c r="O20" s="2">
+        <v>0.93099194486375614</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1.2698705655670761</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>1.1408382282851501</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1.4621176758447383</v>
+      </c>
+      <c r="S20" s="2">
+        <v>1.5374952913338096</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1.723206254479446</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1.6662766112417191</v>
+      </c>
+      <c r="V20" s="2">
+        <v>2.7906761996915677</v>
+      </c>
+      <c r="W20" s="2">
+        <v>4.3567301850333795</v>
+      </c>
+      <c r="X20" s="2">
+        <v>4.1269398854650756</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>4.2516154732797684</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>42380</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.50531574853166739</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.32625491339301937</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.69065804727396951</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.41279837549000487</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.80112790187843275</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.7330270627498463</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.78047802081794515</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.43768588334425751</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.9088896931393318</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.1261324272941589</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.3251319854554489</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1.6700552426902426</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0.78480385210651149</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0.58079355130448795</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1.0932233995819243</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>1.0649708941046792</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1.401095748237815</v>
+      </c>
+      <c r="S21" s="2">
+        <v>1.4776220161875204</v>
+      </c>
+      <c r="T21" s="2">
+        <v>1.4658978657207065</v>
+      </c>
+      <c r="U21" s="2">
+        <v>1.4899703705739502</v>
+      </c>
+      <c r="V21" s="2">
+        <v>3.5803039777799723</v>
+      </c>
+      <c r="W21" s="2">
+        <v>3.9312197925278696</v>
+      </c>
+      <c r="X21" s="2">
+        <v>4.1213161072966313</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>4.3742357697129899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>42383</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.45656999500546191</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.33321904020906035</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.79068115136638206</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.63259259356671271</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.61088826773256411</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.66116287208938951</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.66297226244602236</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.59638241174883344</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.8883444214309371</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.2998111776535202</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.419349882750828</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1.5970205731944473</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0.9305888090041925</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0.73932579805044418</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1.3154972127023934</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>1.2149945467452841</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1.6425375485767471</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1.5165881933530927</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1.558373766481195</v>
+      </c>
+      <c r="U22" s="2">
+        <v>1.5538364442555388</v>
+      </c>
+      <c r="V22" s="2">
+        <v>3.9819878613921347</v>
+      </c>
+      <c r="W22" s="2">
+        <v>4.5110685243051538</v>
+      </c>
+      <c r="X22" s="2">
+        <v>4.8548561820315763</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>4.9673446900478657</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>42388</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.50362051472565506</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.48048639722584852</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.75953644915389162</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.59025178640690279</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.60794393417033288</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.63205253572181885</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.59327487583830896</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.70627694420972253</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.3960023860568742</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.0829746752757974</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.0565932780738869</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1.3026211466751776</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.81335350616632918</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0.77256170406928526</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1.0933446467207861</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1.0059327844400323</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1.4215826099209832</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1.3402173262366297</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1.3411518585440299</v>
+      </c>
+      <c r="U23" s="2">
+        <v>1.2825596531362036</v>
+      </c>
+      <c r="V23" s="2">
+        <v>2.3691471466309215</v>
+      </c>
+      <c r="W23" s="2">
+        <v>3.2542247403516251</v>
+      </c>
+      <c r="X23" s="2">
+        <v>3.7876388601837681</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>3.7938164276318469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>42391</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.5385574192411553</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.45845114363585421</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.76612288845553056</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.70251198492445888</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.75453471145863871</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.68073874423776237</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.81932750328114157</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.66771782362661847</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.7349944186935335</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.2133432886154523</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.2458239065227801</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1.3545061848438404</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0.77506724010691408</v>
+      </c>
+      <c r="O24" s="2">
+        <v>0.86311188122272253</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.99920671465421085</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>0.97708727057419653</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1.54393507379943</v>
+      </c>
+      <c r="S24" s="2">
+        <v>1.2656942508764248</v>
+      </c>
+      <c r="T24" s="2">
+        <v>1.3558992842774824</v>
+      </c>
+      <c r="U24" s="2">
+        <v>1.4547976123188957</v>
+      </c>
+      <c r="V24" s="2">
+        <v>2.3735247798447356</v>
+      </c>
+      <c r="W24" s="2">
+        <v>3.0314388179568743</v>
+      </c>
+      <c r="X24" s="2">
+        <v>3.952928619134763</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>3.8518821287028033</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>42394</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.46316223476719254</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.40086446049981894</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.77554182688840745</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.57939237606142358</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.64740996242754856</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.65596552590449098</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.61998337027851635</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.63721828928040336</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.5172969879435285</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1.1038334688601368</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.1368410418387305</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1.2321521660850585</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.77075375656996514</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.64429652507873281</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.98512128905466712</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.8447190551026541</v>
+      </c>
+      <c r="R25" s="2">
+        <v>1.1559887755289127</v>
+      </c>
+      <c r="S25" s="2">
+        <v>1.0652713901469149</v>
+      </c>
+      <c r="T25" s="2">
+        <v>1.1255493686172149</v>
+      </c>
+      <c r="U25" s="2">
+        <v>1.243282703117381</v>
+      </c>
+      <c r="V25" s="2">
+        <v>2.1148142809566197</v>
+      </c>
+      <c r="W25" s="2">
+        <v>2.8383303036629051</v>
+      </c>
+      <c r="X25" s="2">
+        <v>3.2250147500410238</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>3.43185222061742</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.64867193011528745</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.62071282203817668</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.9855962618418973</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.77531202780838515</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.85751732056938335</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.8762831437269506</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.022036506881679</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.82953321051102158</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.9217566615582133</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1.2316486064094154</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1.4998587079594503</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1.6096791418358478</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0.78137597319704788</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0.94450180411417561</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1.0307824910369165</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0.932849790073913</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1.1946481022685569</v>
+      </c>
+      <c r="S26" s="2">
+        <v>1.4053624270464873</v>
+      </c>
+      <c r="T26" s="2">
+        <v>1.1785065738056013</v>
+      </c>
+      <c r="U26" s="2">
+        <v>1.5183550349299071</v>
+      </c>
+      <c r="V26" s="2">
+        <v>2.2015768417449415</v>
+      </c>
+      <c r="W26" s="2">
+        <v>2.5733555289858301</v>
+      </c>
+      <c r="X26" s="2">
+        <v>2.855502276376876</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>2.9207938331442813</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>42409</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0.62980416345733969</v>
+      </c>
+      <c r="O27" s="2">
+        <v>0.65918048728479928</v>
+      </c>
+      <c r="P27" s="2">
+        <v>0.97644064227217131</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>0.77284411418404031</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1.0607031176246888</v>
+      </c>
+      <c r="S27" s="2">
+        <v>1.0305239366996257</v>
+      </c>
+      <c r="T27" s="2">
+        <v>1.0537541267478712</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0.92580912918036307</v>
+      </c>
+      <c r="V27" s="2">
+        <v>2.0837274132104682</v>
+      </c>
+      <c r="W27" s="2">
+        <v>2.2281688684724577</v>
+      </c>
+      <c r="X27" s="2">
+        <v>2.4361348677848462</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>2.1656497912835029</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>42306</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.35265325992935637</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.40607653061224486</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.93178406361879418</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.95958525905025904</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.42540602159468438</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.58460215472027977</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.44671885853609994</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.52129699248120309</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.89682537319068567</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.93734634026927788</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.88709074100932173</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.50293743663414858</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1.4544301928254675</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0.48824684875183549</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.1423103863324175</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.9472428615962083</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0.87349800537206523</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.51506059674775717</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.4907588533834587</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.44589346938775504</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1.0687417658730156</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1.1415311588541668</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0.61123119443710938</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0.54862046968641121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>42327</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.60643605272532952</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.593942953702292</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.6762574181635053</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.1971208025878652</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.9034919827051342</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.1491159123978656</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.90825846298915613</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.1100693154051597</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2.109773865643175</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.5969697392871227</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2.1330825272898144</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.556089180605547</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2.8827542541758326</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0.92444217469943624</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2.0887186260236583</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1.5317163882117124</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2.4144086250394201</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1.4696789112554112</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1.2415629905031322</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1.0257944983215217</v>
+      </c>
+      <c r="V6" s="2">
+        <v>3.3078241370987209</v>
+      </c>
+      <c r="W6" s="2">
+        <v>3.7951769388391461</v>
+      </c>
+      <c r="X6" s="2">
+        <v>2.3898532567049813</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>2.1185446843853817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>42341</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.42889479762220289</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.5377880234911766</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.2225332199414143</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.85810060150375955</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.88039790324303169</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.1109757731383276</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.875428041793057</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.68673207547169812</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.3544595982142857</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.5494314811338468</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.7738715984533453</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1.4472820549377436</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1.4377603607094418</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.6743081271712813</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1.3065850651525543</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1.3830532341458264</v>
+      </c>
+      <c r="R7" s="2">
+        <v>2.2028259655514506</v>
+      </c>
+      <c r="S7" s="2">
+        <v>1.7405208107805445</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1.2043154671853615</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1.6185342330023984</v>
+      </c>
+      <c r="V7" s="2">
+        <v>2.649739064611325</v>
+      </c>
+      <c r="W7" s="2">
+        <v>5.0333648252592642</v>
+      </c>
+      <c r="X7" s="2">
+        <v>2.5875754603371099</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>2.822798281068525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>42353</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.27048304618539176</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.27093677719008014</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.88835758978259649</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.61657998234452527</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.74464196785743453</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.72400628037511139</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.65718715437788011</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.5738274942711088</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.87742669845053622</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.8113838702033644</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.1434944470514621</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1.3315846890817065</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1.1315513374841462</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.60221628418736239</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1.3899167568347399</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.4864525356075002</v>
+      </c>
+      <c r="R8" s="2">
+        <v>2.695297385220492</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1.3391137982536767</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1.1443585929377498</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1.2751215321324061</v>
+      </c>
+      <c r="V8" s="2">
+        <v>2.6024308139668269</v>
+      </c>
+      <c r="W8" s="2">
+        <v>4.567164444201552</v>
+      </c>
+      <c r="X8" s="2">
+        <v>3.0766429335370509</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>2.8010350814564804</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>42375</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.11105957126148706</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9.5696773161645626E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.14237607061409266</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.16492771627006</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.24574066839940034</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.21012161579765437</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.2312279699992924</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.11346968457447075</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.17001559273410743</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.10315562599323624</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.4414697765723391</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.5239875992063493</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.6094680434066343</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.34108017550685171</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0.81162252875028484</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.69648529240237744</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.85153062296416937</v>
+      </c>
+      <c r="S9" s="2">
+        <v>1.1470741996632787</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.63130900759716513</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1.150724739720788</v>
+      </c>
+      <c r="V9" s="2">
+        <v>2.5959402229725423</v>
+      </c>
+      <c r="W9" s="2">
+        <v>2.7453624181933596</v>
+      </c>
+      <c r="X9" s="2">
+        <v>3.8304429106004796</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>2.4537910725065393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>